<commit_message>
Cambios de index y plataforma
</commit_message>
<xml_diff>
--- a/excel/Vendors-Grafica.xlsx
+++ b/excel/Vendors-Grafica.xlsx
@@ -848,7 +848,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,18 +906,10 @@
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Subida de excel solo
</commit_message>
<xml_diff>
--- a/excel/Vendors-Grafica.xlsx
+++ b/excel/Vendors-Grafica.xlsx
@@ -848,7 +848,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,9 +906,15 @@
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="n">
         <v>1</v>

</xml_diff>